<commit_message>
Tabela Gabarito gerada, biblioteca de QRCODE instalada, mas não está mostrando o QRCode em cada prova.
</commit_message>
<xml_diff>
--- a/questoes.xlsx
+++ b/questoes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="121">
   <si>
     <t>enunciado</t>
   </si>
@@ -55,6 +55,66 @@
     <t>Qual é o valor da raiz quadrada de 144?</t>
   </si>
   <si>
+    <t>Quanto é 7 + 5?</t>
+  </si>
+  <si>
+    <t>Qual é o antônimo de 'feliz'?</t>
+  </si>
+  <si>
+    <t>Qual é o plural de 'cão'?</t>
+  </si>
+  <si>
+    <t>Qual desses animais é um mamífero?</t>
+  </si>
+  <si>
+    <t>Qual é a cor do céu em um dia ensolarado?</t>
+  </si>
+  <si>
+    <t>Qual é a estação do ano mais quente?</t>
+  </si>
+  <si>
+    <t>Em que continente está o Brasil?</t>
+  </si>
+  <si>
+    <t>Quantas patas tem uma aranha?</t>
+  </si>
+  <si>
+    <t>Qual é o número que vem depois do 29?</t>
+  </si>
+  <si>
+    <t>Quem escreveu 'O Sítio do Picapau Amarelo'?</t>
+  </si>
+  <si>
+    <t>Quanto é 1 + 1?</t>
+  </si>
+  <si>
+    <t>Quanto é 2 + 2?</t>
+  </si>
+  <si>
+    <t>Quanto é 3 + 3?</t>
+  </si>
+  <si>
+    <t>Quanto é 4 + 4?</t>
+  </si>
+  <si>
+    <t>Quanto é 5 + 5?</t>
+  </si>
+  <si>
+    <t>Quanto é 6 + 6?</t>
+  </si>
+  <si>
+    <t>Quanto é 7 + 7?</t>
+  </si>
+  <si>
+    <t>Quanto é 8 + 8?</t>
+  </si>
+  <si>
+    <t>Quanto é 9 + 9?</t>
+  </si>
+  <si>
+    <t>Quanto é 10 + 10?</t>
+  </si>
+  <si>
     <t>São Paulo</t>
   </si>
   <si>
@@ -64,6 +124,66 @@
     <t>Eles gostaram da festa.</t>
   </si>
   <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Contente</t>
+  </si>
+  <si>
+    <t>Cães</t>
+  </si>
+  <si>
+    <t>Cobra</t>
+  </si>
+  <si>
+    <t>Verde</t>
+  </si>
+  <si>
+    <t>Outono</t>
+  </si>
+  <si>
+    <t>África</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Monteiro Lobato</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
     <t>Rio de Janeiro</t>
   </si>
   <si>
@@ -73,6 +193,54 @@
     <t>Ela viajou para Paris.</t>
   </si>
   <si>
+    <t>Triste</t>
+  </si>
+  <si>
+    <t>Cãos</t>
+  </si>
+  <si>
+    <t>Jacaré</t>
+  </si>
+  <si>
+    <t>Azul</t>
+  </si>
+  <si>
+    <t>Primavera</t>
+  </si>
+  <si>
+    <t>Ásia</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>Machado de Assis</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
     <t>Brasília</t>
   </si>
   <si>
@@ -82,6 +250,33 @@
     <t>Nós estamos estudando muito.</t>
   </si>
   <si>
+    <t>Alegre</t>
+  </si>
+  <si>
+    <t>Cãoes</t>
+  </si>
+  <si>
+    <t>Sapo</t>
+  </si>
+  <si>
+    <t>Rosa</t>
+  </si>
+  <si>
+    <t>Verão</t>
+  </si>
+  <si>
+    <t>Europa</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>Carlos Drummond</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
     <t>Salvador</t>
   </si>
   <si>
@@ -91,6 +286,30 @@
     <t>A gente vão ao cinema.</t>
   </si>
   <si>
+    <t>Satisfeito</t>
+  </si>
+  <si>
+    <t>Caões</t>
+  </si>
+  <si>
+    <t>Cachorro</t>
+  </si>
+  <si>
+    <t>Preto</t>
+  </si>
+  <si>
+    <t>Inverno</t>
+  </si>
+  <si>
+    <t>Oceania</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>Cecília Meireles</t>
+  </si>
+  <si>
     <t>Fortaleza</t>
   </si>
   <si>
@@ -100,6 +319,30 @@
     <t>O aluno fez a prova.</t>
   </si>
   <si>
+    <t>Radiante</t>
+  </si>
+  <si>
+    <t>Canes</t>
+  </si>
+  <si>
+    <t>Papagaio</t>
+  </si>
+  <si>
+    <t>Amarelo</t>
+  </si>
+  <si>
+    <t>Nenhuma</t>
+  </si>
+  <si>
+    <t>América do Sul</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>Vinícius de Moraes</t>
+  </si>
+  <si>
     <t>Geografia,Português</t>
   </si>
   <si>
@@ -113,6 +356,27 @@
   </si>
   <si>
     <t>Matemática,Ensino Médio</t>
+  </si>
+  <si>
+    <t>Português,Ensino Fundamental</t>
+  </si>
+  <si>
+    <t>Ciências,Natureza</t>
+  </si>
+  <si>
+    <t>Ciências,Ensino Fundamental</t>
+  </si>
+  <si>
+    <t>Geografia,Ensino Fundamental</t>
+  </si>
+  <si>
+    <t>Ciências,Animais</t>
+  </si>
+  <si>
+    <t>Matemática,Números</t>
+  </si>
+  <si>
+    <t>Literatura,Ensino Fundamental</t>
   </si>
 </sst>
 </file>
@@ -470,7 +734,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -507,25 +771,25 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>98</v>
       </c>
       <c r="G2">
         <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -551,7 +815,7 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -559,25 +823,25 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -585,25 +849,25 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>89</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="G5">
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -629,7 +893,527 @@
         <v>2</v>
       </c>
       <c r="H6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" t="s">
+        <v>104</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" t="s">
+        <v>105</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" t="s">
+        <v>106</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15" t="s">
+        <v>107</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" t="s">
+        <v>108</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
         <v>32</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>